<commit_message>
Release v1.0.2: Added Readme.md and Instructions
</commit_message>
<xml_diff>
--- a/examples/data/report.xlsx
+++ b/examples/data/report.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,7 +27,14 @@
     </font>
     <font>
       <b val="1"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
       <color rgb="00FFFFFF"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -48,7 +55,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -77,6 +84,22 @@
       </bottom>
     </border>
     <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="00D9D9D9"/>
       </left>
@@ -108,8 +131,18 @@
       <left style="thin">
         <color rgb="00000000"/>
       </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00D9D9D9"/>
+      </left>
       <right style="thin">
-        <color rgb="00D9D9D9"/>
+        <color rgb="00000000"/>
       </right>
       <top style="thin">
         <color rgb="00000000"/>
@@ -120,13 +153,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="00D9D9D9"/>
       </left>
       <right style="thin">
         <color rgb="00000000"/>
       </right>
       <top style="thin">
-        <color rgb="00000000"/>
+        <color rgb="00D9D9D9"/>
       </top>
       <bottom style="thin">
         <color rgb="00D9D9D9"/>
@@ -136,25 +177,35 @@
       <left style="thin">
         <color rgb="00000000"/>
       </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00D9D9D9"/>
+      </left>
       <right style="thin">
-        <color rgb="00D9D9D9"/>
+        <color rgb="00000000"/>
       </right>
       <top style="thin">
         <color rgb="00D9D9D9"/>
       </top>
       <bottom style="thin">
-        <color rgb="00D9D9D9"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00D9D9D9"/>
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
       </left>
       <right style="thin">
-        <color rgb="00000000"/>
+        <color rgb="00D9D9D9"/>
       </right>
       <top style="thin">
-        <color rgb="00D9D9D9"/>
+        <color rgb="00000000"/>
       </top>
       <bottom style="thin">
         <color rgb="00D9D9D9"/>
@@ -171,15 +222,15 @@
         <color rgb="00D9D9D9"/>
       </top>
       <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="00D9D9D9"/>
+        <color rgb="00D9D9D9"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
       </left>
       <right style="thin">
-        <color rgb="00000000"/>
+        <color rgb="00D9D9D9"/>
       </right>
       <top style="thin">
         <color rgb="00D9D9D9"/>
@@ -187,24 +238,86 @@
       <bottom style="thin">
         <color rgb="00000000"/>
       </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -298,6 +411,31 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>304919</colOff>
+      <row>15</row>
+      <rowOff>90490</rowOff>
+    </from>
+    <ext cx="3048000" cy="2286000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -600,7 +738,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B5:D8"/>
+  <dimension ref="B4:H22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -610,69 +748,297 @@
   <sheetData>
     <row r="1" ht="22" customFormat="1" customHeight="1" s="1"/>
     <row r="2" ht="22" customFormat="1" customHeight="1" s="1"/>
+    <row r="4">
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>with_index</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>without_index</t>
+        </is>
+      </c>
+    </row>
     <row r="5">
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>City</t>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>B</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="D6" s="5" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
+      <c r="B6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <v>1.2</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="6" t="inlineStr">
-        <is>
-          <t>Alice</t>
-        </is>
-      </c>
-      <c r="C7" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D7" s="8" t="inlineStr">
-        <is>
-          <t>London</t>
-        </is>
+      <c r="B7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="10" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G7" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" s="10" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="9" t="inlineStr">
-        <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="C8" s="10" t="n">
-        <v>35</v>
-      </c>
-      <c r="D8" s="11" t="inlineStr">
-        <is>
-          <t>Paris</t>
-        </is>
+      <c r="B8" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G8" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" s="10" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" s="10" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="G9" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" s="10" t="n">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G10" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" s="10" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="H11" s="10" t="n">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C12" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="C13" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" s="14" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G13" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" s="14" t="n">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>with_multiIndex</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="16" t="inlineStr">
+        <is>
+          <t>Group1</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>subgroup1</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="17" t="n"/>
+      <c r="C18" s="9" t="inlineStr">
+        <is>
+          <t>subgroup2</t>
+        </is>
+      </c>
+      <c r="D18" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E18" s="10" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="18" t="inlineStr">
+        <is>
+          <t>Group2</t>
+        </is>
+      </c>
+      <c r="C19" s="9" t="inlineStr">
+        <is>
+          <t>subgroup2</t>
+        </is>
+      </c>
+      <c r="D19" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="10" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="17" t="n"/>
+      <c r="C20" s="9" t="inlineStr">
+        <is>
+          <t>subgroup1</t>
+        </is>
+      </c>
+      <c r="D20" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E20" s="10" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="18" t="inlineStr">
+        <is>
+          <t>Group3</t>
+        </is>
+      </c>
+      <c r="C21" s="9" t="inlineStr">
+        <is>
+          <t>subgroup1</t>
+        </is>
+      </c>
+      <c r="D21" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" s="10" t="n">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" s="19" t="n"/>
+      <c r="C22" s="13" t="inlineStr">
+        <is>
+          <t>subgroup2</t>
+        </is>
+      </c>
+      <c r="D22" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="14" t="n">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B17:B18"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>

</xml_diff>